<commit_message>
Update Map for Site Plan
</commit_message>
<xml_diff>
--- a/Civilworks cost/Slope Protection/Pac-30/Noagan Part-A -Pac-30.xlsx
+++ b/Civilworks cost/Slope Protection/Pac-30/Noagan Part-A -Pac-30.xlsx
@@ -1017,12 +1017,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="15">
@@ -1194,7 +1200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1586,30 +1592,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1628,33 +1655,16 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1982,36 +1992,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="185" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
+      <c r="B1" s="184"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="184"/>
+      <c r="F1" s="184"/>
+      <c r="G1" s="184"/>
+      <c r="H1" s="184"/>
+      <c r="I1" s="184"/>
+      <c r="J1" s="184"/>
+      <c r="K1" s="184"/>
+      <c r="L1" s="184"/>
       <c r="O1" s="26"/>
     </row>
     <row r="2" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="186" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
-      <c r="I2" s="178"/>
+      <c r="C2" s="187"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="1" t="s">
@@ -2022,18 +2032,18 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="173" t="s">
+      <c r="B3" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="179"/>
-      <c r="D3" s="179"/>
-      <c r="E3" s="179"/>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="179"/>
-      <c r="I3" s="179"/>
-      <c r="J3" s="179"/>
-      <c r="K3" s="180"/>
+      <c r="C3" s="175"/>
+      <c r="D3" s="175"/>
+      <c r="E3" s="175"/>
+      <c r="F3" s="175"/>
+      <c r="G3" s="175"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="175"/>
+      <c r="J3" s="175"/>
+      <c r="K3" s="183"/>
       <c r="L3" s="27"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2314,18 +2324,18 @@
       <c r="A16" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="173" t="s">
+      <c r="B16" s="182" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="179"/>
-      <c r="D16" s="179"/>
-      <c r="E16" s="179"/>
-      <c r="F16" s="179"/>
-      <c r="G16" s="179"/>
-      <c r="H16" s="179"/>
-      <c r="I16" s="179"/>
-      <c r="J16" s="179"/>
-      <c r="K16" s="180"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="175"/>
+      <c r="F16" s="175"/>
+      <c r="G16" s="175"/>
+      <c r="H16" s="175"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="183"/>
       <c r="L16" s="28"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2759,18 +2769,18 @@
       <c r="A35" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="173" t="s">
+      <c r="B35" s="182" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="179"/>
-      <c r="D35" s="179"/>
-      <c r="E35" s="179"/>
-      <c r="F35" s="179"/>
-      <c r="G35" s="179"/>
-      <c r="H35" s="179"/>
-      <c r="I35" s="179"/>
-      <c r="J35" s="179"/>
-      <c r="K35" s="180"/>
+      <c r="C35" s="175"/>
+      <c r="D35" s="175"/>
+      <c r="E35" s="175"/>
+      <c r="F35" s="175"/>
+      <c r="G35" s="175"/>
+      <c r="H35" s="175"/>
+      <c r="I35" s="175"/>
+      <c r="J35" s="175"/>
+      <c r="K35" s="183"/>
       <c r="L35" s="28"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2815,18 +2825,18 @@
       <c r="A38" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="173" t="s">
+      <c r="B38" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="179"/>
-      <c r="D38" s="179"/>
-      <c r="E38" s="179"/>
-      <c r="F38" s="179"/>
-      <c r="G38" s="179"/>
-      <c r="H38" s="179"/>
-      <c r="I38" s="179"/>
-      <c r="J38" s="179"/>
-      <c r="K38" s="180"/>
+      <c r="C38" s="175"/>
+      <c r="D38" s="175"/>
+      <c r="E38" s="175"/>
+      <c r="F38" s="175"/>
+      <c r="G38" s="175"/>
+      <c r="H38" s="175"/>
+      <c r="I38" s="175"/>
+      <c r="J38" s="175"/>
+      <c r="K38" s="183"/>
       <c r="L38" s="28"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2871,18 +2881,18 @@
       <c r="A41" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="173" t="s">
+      <c r="B41" s="182" t="s">
         <v>135</v>
       </c>
-      <c r="C41" s="179"/>
-      <c r="D41" s="179"/>
-      <c r="E41" s="179"/>
-      <c r="F41" s="179"/>
-      <c r="G41" s="179"/>
-      <c r="H41" s="179"/>
-      <c r="I41" s="179"/>
-      <c r="J41" s="179"/>
-      <c r="K41" s="180"/>
+      <c r="C41" s="175"/>
+      <c r="D41" s="175"/>
+      <c r="E41" s="175"/>
+      <c r="F41" s="175"/>
+      <c r="G41" s="175"/>
+      <c r="H41" s="175"/>
+      <c r="I41" s="175"/>
+      <c r="J41" s="175"/>
+      <c r="K41" s="183"/>
       <c r="L41" s="28"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3161,18 +3171,18 @@
       <c r="A53" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="B53" s="181" t="s">
+      <c r="B53" s="188" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="182"/>
-      <c r="D53" s="182"/>
-      <c r="E53" s="182"/>
-      <c r="F53" s="182"/>
-      <c r="G53" s="182"/>
-      <c r="H53" s="182"/>
-      <c r="I53" s="182"/>
-      <c r="J53" s="182"/>
-      <c r="K53" s="182"/>
+      <c r="C53" s="189"/>
+      <c r="D53" s="189"/>
+      <c r="E53" s="189"/>
+      <c r="F53" s="189"/>
+      <c r="G53" s="189"/>
+      <c r="H53" s="189"/>
+      <c r="I53" s="189"/>
+      <c r="J53" s="189"/>
+      <c r="K53" s="189"/>
       <c r="L53" s="103"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3536,18 +3546,18 @@
       <c r="A69" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="B69" s="173" t="s">
+      <c r="B69" s="182" t="s">
         <v>88</v>
       </c>
-      <c r="C69" s="174"/>
-      <c r="D69" s="174"/>
-      <c r="E69" s="174"/>
-      <c r="F69" s="174"/>
-      <c r="G69" s="174"/>
-      <c r="H69" s="174"/>
-      <c r="I69" s="174"/>
-      <c r="J69" s="174"/>
-      <c r="K69" s="174"/>
+      <c r="C69" s="176"/>
+      <c r="D69" s="176"/>
+      <c r="E69" s="176"/>
+      <c r="F69" s="176"/>
+      <c r="G69" s="176"/>
+      <c r="H69" s="176"/>
+      <c r="I69" s="176"/>
+      <c r="J69" s="176"/>
+      <c r="K69" s="176"/>
       <c r="L69" s="27"/>
     </row>
     <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3893,13 +3903,13 @@
     </row>
     <row r="83" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="28"/>
-      <c r="B83" s="183" t="s">
+      <c r="B83" s="190" t="s">
         <v>90</v>
       </c>
-      <c r="C83" s="184"/>
-      <c r="D83" s="184"/>
-      <c r="E83" s="184"/>
-      <c r="F83" s="184"/>
+      <c r="C83" s="191"/>
+      <c r="D83" s="191"/>
+      <c r="E83" s="191"/>
+      <c r="F83" s="191"/>
       <c r="G83" s="34">
         <f>K81</f>
         <v>2637.5560000000037</v>
@@ -3940,18 +3950,18 @@
     </row>
     <row r="85" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="28"/>
-      <c r="B85" s="185" t="s">
+      <c r="B85" s="192" t="s">
         <v>91</v>
       </c>
-      <c r="C85" s="186"/>
-      <c r="D85" s="186"/>
-      <c r="E85" s="186"/>
-      <c r="F85" s="186"/>
-      <c r="G85" s="186"/>
-      <c r="H85" s="186"/>
-      <c r="I85" s="186"/>
-      <c r="J85" s="186"/>
-      <c r="K85" s="186"/>
+      <c r="C85" s="193"/>
+      <c r="D85" s="193"/>
+      <c r="E85" s="193"/>
+      <c r="F85" s="193"/>
+      <c r="G85" s="193"/>
+      <c r="H85" s="193"/>
+      <c r="I85" s="193"/>
+      <c r="J85" s="193"/>
+      <c r="K85" s="193"/>
       <c r="L85" s="28"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -3996,18 +4006,18 @@
       <c r="A88" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="B88" s="173" t="s">
+      <c r="B88" s="182" t="s">
         <v>94</v>
       </c>
-      <c r="C88" s="174"/>
-      <c r="D88" s="174"/>
-      <c r="E88" s="174"/>
-      <c r="F88" s="174"/>
-      <c r="G88" s="174"/>
-      <c r="H88" s="174"/>
-      <c r="I88" s="174"/>
-      <c r="J88" s="174"/>
-      <c r="K88" s="174"/>
+      <c r="C88" s="176"/>
+      <c r="D88" s="176"/>
+      <c r="E88" s="176"/>
+      <c r="F88" s="176"/>
+      <c r="G88" s="176"/>
+      <c r="H88" s="176"/>
+      <c r="I88" s="176"/>
+      <c r="J88" s="176"/>
+      <c r="K88" s="176"/>
       <c r="L88" s="27"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
@@ -4374,10 +4384,10 @@
     </row>
     <row r="104" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="69"/>
-      <c r="B104" s="188" t="s">
+      <c r="B104" s="177" t="s">
         <v>103</v>
       </c>
-      <c r="C104" s="189"/>
+      <c r="C104" s="178"/>
       <c r="D104" s="31" t="s">
         <v>104</v>
       </c>
@@ -4479,11 +4489,11 @@
       <c r="A108" s="69"/>
       <c r="B108" s="110"/>
       <c r="C108" s="63"/>
-      <c r="D108" s="190" t="s">
+      <c r="D108" s="179" t="s">
         <v>105</v>
       </c>
-      <c r="E108" s="190"/>
-      <c r="F108" s="190"/>
+      <c r="E108" s="179"/>
+      <c r="F108" s="179"/>
       <c r="G108" s="65">
         <f>SUM(G105:G107)</f>
         <v>1681.0000000000027</v>
@@ -4498,10 +4508,10 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="69"/>
-      <c r="B109" s="188" t="s">
+      <c r="B109" s="177" t="s">
         <v>103</v>
       </c>
-      <c r="C109" s="189"/>
+      <c r="C109" s="178"/>
       <c r="D109" s="31" t="s">
         <v>106</v>
       </c>
@@ -4803,18 +4813,18 @@
       <c r="A122" s="127" t="s">
         <v>113</v>
       </c>
-      <c r="B122" s="191" t="s">
+      <c r="B122" s="180" t="s">
         <v>21</v>
       </c>
-      <c r="C122" s="179"/>
-      <c r="D122" s="179"/>
-      <c r="E122" s="179"/>
-      <c r="F122" s="179"/>
-      <c r="G122" s="179"/>
-      <c r="H122" s="179"/>
-      <c r="I122" s="179"/>
-      <c r="J122" s="179"/>
-      <c r="K122" s="192"/>
+      <c r="C122" s="175"/>
+      <c r="D122" s="175"/>
+      <c r="E122" s="175"/>
+      <c r="F122" s="175"/>
+      <c r="G122" s="175"/>
+      <c r="H122" s="175"/>
+      <c r="I122" s="175"/>
+      <c r="J122" s="175"/>
+      <c r="K122" s="181"/>
       <c r="L122" s="28"/>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
@@ -5111,34 +5121,34 @@
       <c r="A136" s="108" t="s">
         <v>119</v>
       </c>
-      <c r="B136" s="173" t="s">
+      <c r="B136" s="182" t="s">
         <v>152</v>
       </c>
-      <c r="C136" s="179"/>
-      <c r="D136" s="179"/>
-      <c r="E136" s="179"/>
-      <c r="F136" s="179"/>
-      <c r="G136" s="179"/>
-      <c r="H136" s="179"/>
-      <c r="I136" s="179"/>
-      <c r="J136" s="179"/>
-      <c r="K136" s="180"/>
+      <c r="C136" s="175"/>
+      <c r="D136" s="175"/>
+      <c r="E136" s="175"/>
+      <c r="F136" s="175"/>
+      <c r="G136" s="175"/>
+      <c r="H136" s="175"/>
+      <c r="I136" s="175"/>
+      <c r="J136" s="175"/>
+      <c r="K136" s="183"/>
       <c r="L136" s="134"/>
     </row>
     <row r="137" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="134"/>
-      <c r="B137" s="191" t="s">
+      <c r="B137" s="180" t="s">
         <v>133</v>
       </c>
-      <c r="C137" s="176"/>
-      <c r="D137" s="176"/>
-      <c r="E137" s="176"/>
-      <c r="F137" s="176"/>
-      <c r="G137" s="176"/>
-      <c r="H137" s="176"/>
-      <c r="I137" s="176"/>
-      <c r="J137" s="176"/>
-      <c r="K137" s="192"/>
+      <c r="C137" s="184"/>
+      <c r="D137" s="184"/>
+      <c r="E137" s="184"/>
+      <c r="F137" s="184"/>
+      <c r="G137" s="184"/>
+      <c r="H137" s="184"/>
+      <c r="I137" s="184"/>
+      <c r="J137" s="184"/>
+      <c r="K137" s="181"/>
       <c r="L137" s="134"/>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
@@ -5460,18 +5470,18 @@
       <c r="A155" s="108" t="s">
         <v>125</v>
       </c>
-      <c r="B155" s="179" t="s">
+      <c r="B155" s="175" t="s">
         <v>132</v>
       </c>
-      <c r="C155" s="174"/>
-      <c r="D155" s="174"/>
-      <c r="E155" s="174"/>
-      <c r="F155" s="174"/>
-      <c r="G155" s="174"/>
-      <c r="H155" s="174"/>
-      <c r="I155" s="174"/>
-      <c r="J155" s="174"/>
-      <c r="K155" s="174"/>
+      <c r="C155" s="176"/>
+      <c r="D155" s="176"/>
+      <c r="E155" s="176"/>
+      <c r="F155" s="176"/>
+      <c r="G155" s="176"/>
+      <c r="H155" s="176"/>
+      <c r="I155" s="176"/>
+      <c r="J155" s="176"/>
+      <c r="K155" s="176"/>
       <c r="L155" s="27"/>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
@@ -5595,11 +5605,11 @@
       <c r="A161" s="69"/>
       <c r="B161" s="110"/>
       <c r="C161" s="63"/>
-      <c r="D161" s="187" t="s">
+      <c r="D161" s="174" t="s">
         <v>105</v>
       </c>
-      <c r="E161" s="187"/>
-      <c r="F161" s="187"/>
+      <c r="E161" s="174"/>
+      <c r="F161" s="174"/>
       <c r="G161" s="65">
         <f>SUM(G158:G160)</f>
         <v>1681.0000000000027</v>
@@ -5701,18 +5711,18 @@
       <c r="A166" s="108" t="s">
         <v>128</v>
       </c>
-      <c r="B166" s="179" t="s">
+      <c r="B166" s="175" t="s">
         <v>25</v>
       </c>
-      <c r="C166" s="174"/>
-      <c r="D166" s="174"/>
-      <c r="E166" s="174"/>
-      <c r="F166" s="174"/>
-      <c r="G166" s="174"/>
-      <c r="H166" s="174"/>
-      <c r="I166" s="174"/>
-      <c r="J166" s="174"/>
-      <c r="K166" s="174"/>
+      <c r="C166" s="176"/>
+      <c r="D166" s="176"/>
+      <c r="E166" s="176"/>
+      <c r="F166" s="176"/>
+      <c r="G166" s="176"/>
+      <c r="H166" s="176"/>
+      <c r="I166" s="176"/>
+      <c r="J166" s="176"/>
+      <c r="K166" s="176"/>
       <c r="L166" s="27"/>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.25">
@@ -5845,15 +5855,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D161:F161"/>
-    <mergeCell ref="B166:K166"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="D108:F108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B122:K122"/>
-    <mergeCell ref="B136:K136"/>
-    <mergeCell ref="B155:K155"/>
-    <mergeCell ref="B137:K137"/>
     <mergeCell ref="B88:K88"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="B2:I2"/>
@@ -5866,6 +5867,15 @@
     <mergeCell ref="B69:K69"/>
     <mergeCell ref="B83:F83"/>
     <mergeCell ref="B85:K85"/>
+    <mergeCell ref="D161:F161"/>
+    <mergeCell ref="B166:K166"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="D108:F108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B122:K122"/>
+    <mergeCell ref="B136:K136"/>
+    <mergeCell ref="B155:K155"/>
+    <mergeCell ref="B137:K137"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5890,14 +5900,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="193" t="s">
+      <c r="A2" s="194" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="193"/>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="193"/>
-      <c r="F2" s="193"/>
+      <c r="B2" s="194"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="194"/>
+      <c r="E2" s="194"/>
+      <c r="F2" s="194"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
@@ -6442,10 +6452,10 @@
       <c r="A28" s="12"/>
       <c r="B28" s="13"/>
       <c r="C28" s="15"/>
-      <c r="D28" s="194" t="s">
+      <c r="D28" s="195" t="s">
         <v>131</v>
       </c>
-      <c r="E28" s="194"/>
+      <c r="E28" s="195"/>
       <c r="F28" s="140">
         <f>SUM(F5:F27)</f>
         <v>146983173.23623323</v>
@@ -6674,7 +6684,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6686,132 +6696,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="196" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="169" t="s">
+      <c r="B1" s="196" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="169">
+      <c r="C1" s="196">
         <v>12.43</v>
       </c>
-      <c r="D1" s="169" t="s">
+      <c r="D1" s="196" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="169">
+      <c r="E1" s="196">
         <v>12.481</v>
       </c>
-      <c r="F1" s="169" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="169">
+      <c r="F1" s="196" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="196">
         <v>51.000000000000156</v>
       </c>
-      <c r="H1" s="168" t="s">
+      <c r="H1" s="197" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="169" t="s">
+      <c r="A2" s="196" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="196" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="169">
+      <c r="C2" s="196">
         <v>19.59</v>
       </c>
-      <c r="D2" s="169" t="s">
+      <c r="D2" s="196" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="169">
+      <c r="E2" s="196">
         <v>20.100000000000001</v>
       </c>
-      <c r="F2" s="169" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="169">
+      <c r="F2" s="196" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="196">
         <v>510.00000000000159</v>
       </c>
-      <c r="H2" s="168" t="s">
+      <c r="H2" s="197" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="169" t="s">
+      <c r="A3" s="196" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="196" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="169">
+      <c r="C3" s="196">
         <v>20.13</v>
       </c>
-      <c r="D3" s="169" t="s">
+      <c r="D3" s="196" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="169">
+      <c r="E3" s="196">
         <v>21.25</v>
       </c>
-      <c r="F3" s="169" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="169">
+      <c r="F3" s="196" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="196">
         <v>1120.0000000000009</v>
       </c>
-      <c r="H3" s="168" t="s">
+      <c r="H3" s="197" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="169" t="s">
+      <c r="A4" s="196" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="169" t="s">
+      <c r="B4" s="196" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="169">
+      <c r="C4" s="196">
         <v>21.95</v>
       </c>
-      <c r="D4" s="169" t="s">
+      <c r="D4" s="196" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="169">
+      <c r="E4" s="196">
         <v>22.69</v>
       </c>
-      <c r="F4" s="169" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="169">
+      <c r="F4" s="196" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="196">
         <v>740.00000000000205</v>
       </c>
-      <c r="H4" s="168" t="s">
+      <c r="H4" s="197" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="169" t="s">
+      <c r="A5" s="196" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="196" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="169">
+      <c r="C5" s="196">
         <v>26.08</v>
       </c>
-      <c r="D5" s="169" t="s">
+      <c r="D5" s="196" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="169">
+      <c r="E5" s="196">
         <v>26.18</v>
       </c>
-      <c r="F5" s="169" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="169">
+      <c r="F5" s="196" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="196">
         <v>100.00000000000142</v>
       </c>
-      <c r="H5" s="168" t="s">
+      <c r="H5" s="197" t="s">
         <v>159</v>
       </c>
     </row>
@@ -7284,7 +7294,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="195" t="s">
+      <c r="A24" s="173" t="s">
         <v>168</v>
       </c>
       <c r="B24" s="168" t="s">

</xml_diff>